<commit_message>
Starting example of Test Case 1: Register User
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\DemoClassAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B6A20E-B642-458D-A885-B85508361194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98352A1D-0EE0-4A6D-ADD0-B1A49AB676A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>email</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>daniel.wilson@example.com</t>
+  </si>
+  <si>
+    <t>avi@testmail.com</t>
   </si>
 </sst>
 </file>
@@ -373,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,37 +393,42 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="mailto:alex.jones@example.com" xr:uid="{AA7548E1-0E77-443F-B673-0A07068A968B}"/>
-    <hyperlink ref="A3" r:id="rId2" display="mailto:samantha.smith@example.com" xr:uid="{86473305-DA47-4C12-B486-47C9C41D3944}"/>
-    <hyperlink ref="A4" r:id="rId3" display="mailto:michael.brown@example.com" xr:uid="{9EFAB206-5D4A-4A02-BCBB-47E8B7105669}"/>
-    <hyperlink ref="A5" r:id="rId4" display="mailto:jessica.davis@example.com" xr:uid="{983160CD-5AA7-4F59-8095-4D12249A3F53}"/>
-    <hyperlink ref="A6" r:id="rId5" display="mailto:daniel.wilson@example.com" xr:uid="{EC53E284-FAE0-4DD6-A1BE-53EF38285BA1}"/>
+    <hyperlink ref="A3" r:id="rId1" display="mailto:alex.jones@example.com" xr:uid="{AA7548E1-0E77-443F-B673-0A07068A968B}"/>
+    <hyperlink ref="A4" r:id="rId2" display="mailto:samantha.smith@example.com" xr:uid="{86473305-DA47-4C12-B486-47C9C41D3944}"/>
+    <hyperlink ref="A5" r:id="rId3" display="mailto:michael.brown@example.com" xr:uid="{9EFAB206-5D4A-4A02-BCBB-47E8B7105669}"/>
+    <hyperlink ref="A6" r:id="rId4" display="mailto:jessica.davis@example.com" xr:uid="{983160CD-5AA7-4F59-8095-4D12249A3F53}"/>
+    <hyperlink ref="A7" r:id="rId5" display="mailto:daniel.wilson@example.com" xr:uid="{EC53E284-FAE0-4DD6-A1BE-53EF38285BA1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>